<commit_message>
kaggle house price predict -  feature enginner
</commit_message>
<xml_diff>
--- a/kaggle/House_Price_Linear_Regression/特征分析.xlsx
+++ b/kaggle/House_Price_Linear_Regression/特征分析.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="16545" windowHeight="11580"/>
+    <workbookView windowWidth="17700" windowHeight="11580"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127">
   <si>
     <t>feature</t>
   </si>
@@ -296,6 +296,105 @@
   </si>
   <si>
     <t>有没有中央空调。这个很重要，但和年限有关吧。比如新房子会有中央空调，旧房子就没有。</t>
+  </si>
+  <si>
+    <t>Electrical</t>
+  </si>
+  <si>
+    <t>供电系统情况</t>
+  </si>
+  <si>
+    <t>1stFlrSF</t>
+  </si>
+  <si>
+    <t>空间、建筑</t>
+  </si>
+  <si>
+    <t>一楼的面积</t>
+  </si>
+  <si>
+    <t>2ndFlrSF</t>
+  </si>
+  <si>
+    <t>二楼面积</t>
+  </si>
+  <si>
+    <t>LowQualFinSF</t>
+  </si>
+  <si>
+    <t>低质量成品的面积，破破烂烂的面积</t>
+  </si>
+  <si>
+    <t>GrLivArea</t>
+  </si>
+  <si>
+    <t>空间/建筑</t>
+  </si>
+  <si>
+    <t>地面上居住总面积，应该重要吧</t>
+  </si>
+  <si>
+    <t>BsmtFullBath</t>
+  </si>
+  <si>
+    <t>地下室的浴室个数（带浴缸类型）</t>
+  </si>
+  <si>
+    <t>BsmtHalfBath</t>
+  </si>
+  <si>
+    <t>地下室的浴室个数（不带浴缸类型）</t>
+  </si>
+  <si>
+    <t>FullBath</t>
+  </si>
+  <si>
+    <t>地上浴室个数（带浴缸类型）</t>
+  </si>
+  <si>
+    <t>HalfBath</t>
+  </si>
+  <si>
+    <t>地上浴室个数（不带浴缸类型）</t>
+  </si>
+  <si>
+    <t>BedroomAbvGr</t>
+  </si>
+  <si>
+    <t>地上卧室个数</t>
+  </si>
+  <si>
+    <t>KitchenAbvGr</t>
+  </si>
+  <si>
+    <t>地上厨房个数</t>
+  </si>
+  <si>
+    <t>TotRmsAbvGrd</t>
+  </si>
+  <si>
+    <t>地上房间个数</t>
+  </si>
+  <si>
+    <t>Firplaces</t>
+  </si>
+  <si>
+    <t>壁炉个数</t>
+  </si>
+  <si>
+    <t>GarageYrBlt</t>
+  </si>
+  <si>
+    <t>车库年限</t>
+  </si>
+  <si>
+    <t>GarageCars</t>
+  </si>
+  <si>
+    <t>车库能停车的数量</t>
+  </si>
+  <si>
+    <t>GarageArea</t>
   </si>
 </sst>
 </file>
@@ -303,10 +402,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -317,24 +416,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -348,7 +431,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -362,32 +452,41 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -408,30 +507,7 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -454,12 +530,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -470,55 +569,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -530,13 +719,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -548,109 +737,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -664,17 +763,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -690,26 +783,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -761,6 +834,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -769,10 +868,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -781,19 +880,19 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -802,112 +901,112 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1234,10 +1333,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
@@ -2073,6 +2172,308 @@
         <v>93</v>
       </c>
     </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>94</v>
+      </c>
+      <c r="B42" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" t="s">
+        <v>23</v>
+      </c>
+      <c r="E42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F42" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>96</v>
+      </c>
+      <c r="B43" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" t="s">
+        <v>97</v>
+      </c>
+      <c r="E43" t="s">
+        <v>15</v>
+      </c>
+      <c r="F43" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>99</v>
+      </c>
+      <c r="B44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" t="s">
+        <v>18</v>
+      </c>
+      <c r="E44" t="s">
+        <v>15</v>
+      </c>
+      <c r="F44" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>101</v>
+      </c>
+      <c r="B45" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" t="s">
+        <v>23</v>
+      </c>
+      <c r="E45" t="s">
+        <v>15</v>
+      </c>
+      <c r="F45" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
+        <v>103</v>
+      </c>
+      <c r="B46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" t="s">
+        <v>104</v>
+      </c>
+      <c r="E46" t="s">
+        <v>15</v>
+      </c>
+      <c r="F46" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" t="s">
+        <v>106</v>
+      </c>
+      <c r="B47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" t="s">
+        <v>23</v>
+      </c>
+      <c r="E47" t="s">
+        <v>11</v>
+      </c>
+      <c r="F47" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" t="s">
+        <v>108</v>
+      </c>
+      <c r="B48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" t="s">
+        <v>23</v>
+      </c>
+      <c r="E48" t="s">
+        <v>11</v>
+      </c>
+      <c r="F48" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
+        <v>110</v>
+      </c>
+      <c r="B49" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" t="s">
+        <v>23</v>
+      </c>
+      <c r="E49" t="s">
+        <v>11</v>
+      </c>
+      <c r="F49" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
+        <v>112</v>
+      </c>
+      <c r="B50" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" t="s">
+        <v>23</v>
+      </c>
+      <c r="E50" t="s">
+        <v>11</v>
+      </c>
+      <c r="F50" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
+        <v>114</v>
+      </c>
+      <c r="B51" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" t="s">
+        <v>23</v>
+      </c>
+      <c r="E51" t="s">
+        <v>11</v>
+      </c>
+      <c r="F51" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" t="s">
+        <v>116</v>
+      </c>
+      <c r="B52" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" t="s">
+        <v>8</v>
+      </c>
+      <c r="D52" t="s">
+        <v>23</v>
+      </c>
+      <c r="E52" t="s">
+        <v>15</v>
+      </c>
+      <c r="F52" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" t="s">
+        <v>118</v>
+      </c>
+      <c r="B53" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" t="s">
+        <v>18</v>
+      </c>
+      <c r="E53" t="s">
+        <v>15</v>
+      </c>
+      <c r="F53" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" t="s">
+        <v>120</v>
+      </c>
+      <c r="B54" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" t="s">
+        <v>23</v>
+      </c>
+      <c r="E54" t="s">
+        <v>15</v>
+      </c>
+      <c r="F54" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" t="s">
+        <v>122</v>
+      </c>
+      <c r="B55" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" t="s">
+        <v>8</v>
+      </c>
+      <c r="D55" t="s">
+        <v>23</v>
+      </c>
+      <c r="E55" t="s">
+        <v>15</v>
+      </c>
+      <c r="F55" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" t="s">
+        <v>124</v>
+      </c>
+      <c r="B56" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56" t="s">
+        <v>18</v>
+      </c>
+      <c r="E56" t="s">
+        <v>11</v>
+      </c>
+      <c r="F56" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>126</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>